<commit_message>
adds location data from katie
</commit_message>
<xml_diff>
--- a/data-raw/metadata/locations_lookup_metadata.xlsx
+++ b/data-raw/metadata/locations_lookup_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/edi-feather-snorkel/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECACFB88-C55F-F34B-BFC3-A142662FA344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5358D0-7EFA-2146-979B-B4A80FF3F281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29700" yWindow="500" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29700" yWindow="500" windowWidth="29480" windowHeight="27120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -91,24 +91,6 @@
     <t>section_type</t>
   </si>
   <si>
-    <t>section_number</t>
-  </si>
-  <si>
-    <t>ordinal</t>
-  </si>
-  <si>
-    <t>snorkel_survey</t>
-  </si>
-  <si>
-    <t>Location were snorkel data was collected.</t>
-  </si>
-  <si>
-    <t>Survey site type. Site types include: permanent - site surveyed repetedly, Random - site surveyed as a proxy if "permanent site" not feasible to survey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number corresponding to section name. </t>
-  </si>
-  <si>
     <t>river_mile</t>
   </si>
   <si>
@@ -116,9 +98,6 @@
   </si>
   <si>
     <t xml:space="preserve">Unit associated with specific record observed </t>
-  </si>
-  <si>
-    <t xml:space="preserve">River mile associated with specific record observed </t>
   </si>
   <si>
     <t>channel_type</t>
@@ -133,9 +112,6 @@
     <t>interval</t>
   </si>
   <si>
-    <t>mini-snorkel-survey</t>
-  </si>
-  <si>
     <t>numeric</t>
   </si>
   <si>
@@ -145,18 +121,41 @@
     <t>real</t>
   </si>
   <si>
-    <t>Longitude of the survey location reported in decimal degrees</t>
+    <t>unit_sub_level</t>
   </si>
   <si>
-    <t>Latitude of the survey location reported in decimal degrees</t>
+    <t>Sub-level associated with a unit. In some cases unit are broken down into two. Levels = c("A", "B", NA)</t>
+  </si>
+  <si>
+    <t>Survey site type. Site types include: permanent - site surveyed repetedly, Random - site surveyed as a proxy if "permanent site" not feasible to survey. When the section type was not included we assumed it was "random"</t>
+  </si>
+  <si>
+    <t>area_sq_m</t>
+  </si>
+  <si>
+    <t>square meters</t>
+  </si>
+  <si>
+    <t>River mile associated with specific record observed as recorded by the survey crew.</t>
+  </si>
+  <si>
+    <t>Latitude of the survey unit reported in decimal degrees. Units were originally manually mapped and were then digitized. The latitude and longitude represent the centroid of the unit. In the few cases where units were unable to be digitized, the latitude and longitude is associated with the river mile location.</t>
+  </si>
+  <si>
+    <t>Longitude of the survey location reported in decimal degrees. Units were originally manually mapped and were then digitized. The latitude and longitude represent the centroid of the unit. In the few cases where units were unable to be digitized, the latitude and longitude is associated with the river mile location.</t>
+  </si>
+  <si>
+    <t>Name associated with the unit and location of the survey. Section names do not exist for all units.</t>
+  </si>
+  <si>
+    <t>This represents the area of the unit in square meters. This was calculated in ArcMap during the unit digitization process.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
@@ -218,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -245,9 +244,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -472,19 +468,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z979"/>
+  <dimension ref="A1:Z980"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
-    <col min="2" max="2" width="42" style="14" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42" style="13" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" customWidth="1"/>
     <col min="6" max="6" width="5.33203125" customWidth="1"/>
     <col min="7" max="7" width="7.1640625" customWidth="1"/>
@@ -552,17 +548,15 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
@@ -572,7 +566,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="5"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="7"/>
+      <c r="L2" s="10"/>
       <c r="M2" s="3"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -590,17 +584,15 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
@@ -608,9 +600,9 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="3"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="10"/>
       <c r="M3" s="3"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -628,17 +620,15 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
@@ -648,7 +638,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="5"/>
       <c r="K4" s="6"/>
-      <c r="L4" s="10"/>
+      <c r="L4" s="7"/>
       <c r="M4" s="3"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -666,17 +656,15 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
@@ -684,10 +672,10 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="3"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -704,17 +692,15 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
@@ -722,9 +708,9 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="10"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -742,17 +728,15 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
@@ -780,37 +764,35 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="H8" s="3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="15">
-        <v>39.316670000000002</v>
+      <c r="J8" s="5"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="10">
+        <v>559.38350000000003</v>
       </c>
-      <c r="M8" s="15">
-        <v>39.516019999999997</v>
+      <c r="M8" s="3">
+        <v>67118.94</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -828,37 +810,35 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="3"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="3">
-        <v>-121.639</v>
+      <c r="L9" s="14">
+        <v>39.316670000000002</v>
       </c>
-      <c r="M9" s="3">
-        <v>-121.5535</v>
+      <c r="M9" s="14">
+        <v>39.516019999999997</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -875,19 +855,37 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="A10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="I10" s="2"/>
       <c r="J10" s="3"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
+      <c r="L10" s="3">
+        <v>-121.639</v>
+      </c>
+      <c r="M10" s="3">
+        <v>-121.5535</v>
+      </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -903,6 +901,16 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="3"/>
       <c r="K11" s="2"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
@@ -921,16 +929,6 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="3"/>
       <c r="K12" s="2"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -1061,6 +1059,7 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
@@ -1088,7 +1087,6 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
@@ -1116,6 +1114,7 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
@@ -1143,7 +1142,6 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>
@@ -2095,7 +2093,7 @@
       <c r="Z53" s="1"/>
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="1"/>
+      <c r="A54" s="4"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="2"/>
@@ -28022,18 +28020,46 @@
       <c r="Y979" s="1"/>
       <c r="Z979" s="1"/>
     </row>
+    <row r="980" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A980" s="1"/>
+      <c r="B980" s="1"/>
+      <c r="C980" s="1"/>
+      <c r="D980" s="2"/>
+      <c r="E980" s="1"/>
+      <c r="F980" s="3"/>
+      <c r="G980" s="3"/>
+      <c r="H980" s="3"/>
+      <c r="I980" s="2"/>
+      <c r="J980" s="3"/>
+      <c r="K980" s="2"/>
+      <c r="L980" s="3"/>
+      <c r="M980" s="3"/>
+      <c r="N980" s="1"/>
+      <c r="O980" s="1"/>
+      <c r="P980" s="1"/>
+      <c r="Q980" s="1"/>
+      <c r="R980" s="1"/>
+      <c r="S980" s="1"/>
+      <c r="T980" s="1"/>
+      <c r="U980" s="1"/>
+      <c r="V980" s="1"/>
+      <c r="W980" s="1"/>
+      <c r="X980" s="1"/>
+      <c r="Y980" s="1"/>
+      <c r="Z980" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C36:C979 C12:C24 C1:C10" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C37:C980 C13:C25 C7:C11 C1:C6" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E12:E979 E1:E10" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E13:E980 E7:E11 E1:E6" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F12:F979 F1:F10" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F13:F980 F7:F11 F1:F6" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H12:H979 H1:H10" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H13:H980 H7:H11 H1:H6" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>
@@ -28123,7 +28149,7 @@
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="13"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>

</xml_diff>

<commit_message>
update to unit_sub_level description in metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/locations_lookup_metadata.xlsx
+++ b/data-raw/metadata/locations_lookup_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/edi-feather-snorkel/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/VA/edi-feather-snorkel/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4E405F-3A72-4148-924E-ACE166718EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F77002-4E7A-5D49-94F4-8B06D5CCA55F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29700" yWindow="500" windowWidth="29480" windowHeight="27120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29700" yWindow="500" windowWidth="29480" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -118,9 +118,6 @@
     <t>unit_sub_level</t>
   </si>
   <si>
-    <t>Sub-level associated with a unit. In some cases unit are broken down into two. Levels = c("A", "B", NA)</t>
-  </si>
-  <si>
     <t>area_sq_m</t>
   </si>
   <si>
@@ -137,6 +134,9 @@
   </si>
   <si>
     <t>This represents the area of the unit in square meters. This was calculated in ArcMap during the unit digitization process.</t>
+  </si>
+  <si>
+    <t>Sub-level associated with a unit and with a unique latitude and longitude. In some cases the unit is broken down into two which is a legacy of when the unts were originally mapped. Levels = c("A", "B", NA)</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -572,7 +572,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
@@ -644,7 +644,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -677,10 +677,10 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>25</v>
@@ -693,7 +693,7 @@
         <v>25</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>28</v>
@@ -726,7 +726,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>25</v>
@@ -772,7 +772,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>25</v>

</xml_diff>